<commit_message>
results exp1, 30 tasks
</commit_message>
<xml_diff>
--- a/lab4/results.xlsx
+++ b/lab4/results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jean-Thomas\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jean-Thomas\Documents\EPFL\IntelligentAgents\group_labs\IntelligentAgents\lab4\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
   <si>
     <t>pmin</t>
   </si>
@@ -106,19 +106,10 @@
   <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -146,13 +137,22 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -469,18 +469,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="6" max="6" width="10.6640625" style="4"/>
+    <col min="6" max="6" width="10.6640625" style="3"/>
+    <col min="7" max="7" width="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -496,361 +497,590 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A2" s="5">
+      <c r="G1">
+        <v>30</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A2" s="4">
         <v>0.7</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="4">
         <v>0.1</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="4">
         <v>9347</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="4">
         <v>52149</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="4">
         <f>AVERAGE(C2:C7)</f>
         <v>10095.5</v>
       </c>
-      <c r="F2" s="20">
+      <c r="F2" s="17">
         <f>AVERAGE(D2:D7)</f>
         <v>38153.5</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7">
+      <c r="H2" s="4">
+        <v>12481</v>
+      </c>
+      <c r="I2" s="4">
+        <v>302023</v>
+      </c>
+      <c r="J2" s="4">
+        <f>AVERAGE(H2:H7)</f>
+        <v>13382.833333333334</v>
+      </c>
+      <c r="K2" s="17">
+        <f>AVERAGE(I2:I7)</f>
+        <v>209973.66666666666</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5">
         <v>9347</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="5">
         <v>38269</v>
       </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="16"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7">
+      <c r="E3" s="5"/>
+      <c r="F3" s="13"/>
+      <c r="H3" s="5">
+        <v>15392</v>
+      </c>
+      <c r="I3" s="5">
+        <v>206155</v>
+      </c>
+      <c r="J3" s="5"/>
+      <c r="K3" s="13"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5">
         <v>9653</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="5">
         <v>38512</v>
       </c>
-      <c r="E4" s="7"/>
-      <c r="F4" s="16"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="17">
+      <c r="E4" s="5"/>
+      <c r="F4" s="13"/>
+      <c r="H4" s="5">
+        <v>12992</v>
+      </c>
+      <c r="I4" s="5">
+        <v>302013</v>
+      </c>
+      <c r="J4" s="5"/>
+      <c r="K4" s="13"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="14">
         <v>11662</v>
       </c>
-      <c r="D5" s="17">
+      <c r="D5" s="14">
         <v>23365</v>
       </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="16"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="17">
+      <c r="E5" s="5"/>
+      <c r="F5" s="13"/>
+      <c r="H5" s="14">
+        <v>13599</v>
+      </c>
+      <c r="I5" s="14">
+        <v>93900</v>
+      </c>
+      <c r="J5" s="5"/>
+      <c r="K5" s="13"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="14">
         <v>10375</v>
       </c>
-      <c r="D6" s="17">
+      <c r="D6" s="14">
         <v>32019</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="16"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9">
+      <c r="E6" s="5"/>
+      <c r="F6" s="13"/>
+      <c r="H6" s="14">
+        <v>11559</v>
+      </c>
+      <c r="I6" s="14">
+        <v>232472</v>
+      </c>
+      <c r="J6" s="5"/>
+      <c r="K6" s="13"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6">
         <v>10189</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="6">
         <v>44607</v>
       </c>
-      <c r="E7" s="9"/>
-      <c r="F7" s="10"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="E7" s="6"/>
+      <c r="F7" s="7"/>
+      <c r="H7" s="6">
+        <v>14274</v>
+      </c>
+      <c r="I7" s="6">
+        <v>123279</v>
+      </c>
+      <c r="J7" s="6"/>
+      <c r="K7" s="7"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>0.5</v>
       </c>
       <c r="B8">
         <v>0.3</v>
       </c>
-      <c r="C8" s="17">
+      <c r="C8" s="14">
         <v>9653</v>
       </c>
-      <c r="D8" s="17">
+      <c r="D8" s="14">
         <v>39538</v>
       </c>
       <c r="E8">
         <f>AVERAGE(C8:C13)</f>
         <v>9660.8333333333339</v>
       </c>
-      <c r="F8" s="20">
+      <c r="F8" s="17">
         <f>AVERAGE(D8:D13)</f>
         <v>32936</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="C9" s="17">
+      <c r="H8" s="14">
+        <v>13964</v>
+      </c>
+      <c r="I8" s="14">
+        <v>258058</v>
+      </c>
+      <c r="J8">
+        <f>AVERAGE(H8:H13)</f>
+        <v>13567.166666666666</v>
+      </c>
+      <c r="K8" s="17">
+        <f>AVERAGE(I8:I13)</f>
+        <v>200463.66666666666</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="C9" s="14">
         <v>9347</v>
       </c>
-      <c r="D9" s="17">
+      <c r="D9" s="14">
         <v>24197</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="C10" s="17">
+      <c r="H9" s="14">
+        <v>12993</v>
+      </c>
+      <c r="I9" s="14">
+        <v>227694</v>
+      </c>
+      <c r="K9" s="3"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="C10" s="14">
         <v>9347</v>
       </c>
-      <c r="D10" s="17">
+      <c r="D10" s="14">
         <v>46860</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="C11" s="17">
+      <c r="H10" s="14">
+        <v>14176</v>
+      </c>
+      <c r="I10" s="14">
+        <v>117020</v>
+      </c>
+      <c r="K10" s="3"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="C11" s="14">
         <v>10924</v>
       </c>
-      <c r="D11" s="17">
+      <c r="D11" s="14">
         <v>32943</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="C12" s="17">
+      <c r="H11" s="14">
+        <v>13327</v>
+      </c>
+      <c r="I11" s="14">
+        <v>194495</v>
+      </c>
+      <c r="K11" s="3"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="C12" s="14">
         <v>9347</v>
       </c>
-      <c r="D12" s="17">
+      <c r="D12" s="14">
         <v>23805</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="C13" s="17">
+      <c r="H12" s="14">
+        <v>14492</v>
+      </c>
+      <c r="I12" s="14">
+        <v>165312</v>
+      </c>
+      <c r="K12" s="3"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="C13" s="14">
         <v>9347</v>
       </c>
-      <c r="D13" s="17">
+      <c r="D13" s="14">
         <v>30273</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A14" s="11">
+      <c r="H13" s="14">
+        <v>12451</v>
+      </c>
+      <c r="I13" s="14">
+        <v>240203</v>
+      </c>
+      <c r="K13" s="3"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A14" s="8">
         <v>0.3</v>
       </c>
-      <c r="B14" s="11">
+      <c r="B14" s="8">
         <v>0.5</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="4">
         <v>10924</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="4">
         <v>22968</v>
       </c>
-      <c r="E14" s="18">
+      <c r="E14" s="15">
         <f>AVERAGE(C14:C19)</f>
         <v>9959.5</v>
       </c>
-      <c r="F14" s="20">
+      <c r="F14" s="17">
         <f>AVERAGE(D14:D19)</f>
         <v>32248</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7">
+      <c r="H14" s="4">
+        <v>16693</v>
+      </c>
+      <c r="I14" s="4">
+        <v>150882</v>
+      </c>
+      <c r="J14" s="15">
+        <f>AVERAGE(H14:H19)</f>
+        <v>14325.166666666666</v>
+      </c>
+      <c r="K14" s="17">
+        <f>AVERAGE(I14:I19)</f>
+        <v>161027.66666666666</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5">
         <v>9653</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D15" s="5">
         <v>22893</v>
       </c>
-      <c r="E15" s="19"/>
-      <c r="F15" s="21"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7">
+      <c r="E15" s="16"/>
+      <c r="F15" s="18"/>
+      <c r="H15" s="5">
+        <v>13659</v>
+      </c>
+      <c r="I15" s="5">
+        <v>220823</v>
+      </c>
+      <c r="J15" s="16"/>
+      <c r="K15" s="18"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5">
         <v>9653</v>
       </c>
-      <c r="D16" s="7">
+      <c r="D16" s="5">
         <v>60912</v>
       </c>
-      <c r="E16" s="19"/>
-      <c r="F16" s="21"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7">
+      <c r="E16" s="16"/>
+      <c r="F16" s="18"/>
+      <c r="H16" s="5">
+        <v>14627</v>
+      </c>
+      <c r="I16" s="5">
+        <v>137242</v>
+      </c>
+      <c r="J16" s="16"/>
+      <c r="K16" s="18"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5">
         <v>9347</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="5">
         <v>26067</v>
       </c>
-      <c r="E17" s="12"/>
-      <c r="F17" s="13"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7">
+      <c r="E17" s="9"/>
+      <c r="F17" s="10"/>
+      <c r="H17" s="14">
+        <v>13744</v>
+      </c>
+      <c r="I17" s="14">
+        <v>151764</v>
+      </c>
+      <c r="J17" s="9"/>
+      <c r="K17" s="10"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5">
         <v>10833</v>
       </c>
-      <c r="D18" s="7">
+      <c r="D18" s="5">
         <v>25237</v>
       </c>
-      <c r="E18" s="12"/>
-      <c r="F18" s="13"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A19" s="9"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="9">
+      <c r="E18" s="9"/>
+      <c r="F18" s="10"/>
+      <c r="H18" s="14">
+        <v>13484</v>
+      </c>
+      <c r="I18" s="14">
+        <v>189297</v>
+      </c>
+      <c r="J18" s="9"/>
+      <c r="K18" s="10"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6">
         <v>9347</v>
       </c>
-      <c r="D19" s="9">
+      <c r="D19" s="6">
         <v>35411</v>
       </c>
-      <c r="E19" s="14"/>
-      <c r="F19" s="15"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="E19" s="11"/>
+      <c r="F19" s="12"/>
+      <c r="H19" s="6">
+        <v>13744</v>
+      </c>
+      <c r="I19" s="6">
+        <v>116158</v>
+      </c>
+      <c r="J19" s="11"/>
+      <c r="K19" s="12"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>0.4</v>
       </c>
       <c r="B20">
         <v>0.4</v>
       </c>
-      <c r="C20" s="17">
+      <c r="C20" s="14">
         <v>9653</v>
       </c>
-      <c r="D20" s="17">
+      <c r="D20" s="14">
         <v>28665</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20" s="23">
         <f>AVERAGE(C20:C25)</f>
         <v>9619.8333333333339</v>
       </c>
-      <c r="F20" s="22">
-        <v>32248</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="C21" s="17">
+      <c r="F20" s="24">
+        <f>AVERAGE(D20:D25)</f>
+        <v>37950.833333333336</v>
+      </c>
+      <c r="H20" s="14">
+        <v>13428</v>
+      </c>
+      <c r="I20" s="14">
+        <v>268140</v>
+      </c>
+      <c r="J20" s="23">
+        <f>AVERAGE(H20:H25)</f>
+        <v>13714.666666666666</v>
+      </c>
+      <c r="K20" s="24">
+        <f>AVERAGE(I20:I25)</f>
+        <v>227860.16666666666</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="C21" s="14">
         <v>9347</v>
       </c>
-      <c r="D21" s="17">
+      <c r="D21" s="14">
         <v>28700</v>
       </c>
-      <c r="E21" s="2"/>
-      <c r="F21" s="22"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="C22" s="17">
+      <c r="E21" s="23"/>
+      <c r="F21" s="24"/>
+      <c r="H21" s="14">
+        <v>13345</v>
+      </c>
+      <c r="I21" s="14">
+        <v>267606</v>
+      </c>
+      <c r="J21" s="23"/>
+      <c r="K21" s="24"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="C22" s="14">
         <v>9653</v>
       </c>
-      <c r="D22" s="17">
+      <c r="D22" s="14">
         <v>63159</v>
       </c>
-      <c r="E22" s="2"/>
-      <c r="F22" s="22"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="C23" s="17">
+      <c r="E22" s="23"/>
+      <c r="F22" s="24"/>
+      <c r="H22" s="14">
+        <v>15144</v>
+      </c>
+      <c r="I22" s="14">
+        <v>220307</v>
+      </c>
+      <c r="J22" s="23"/>
+      <c r="K22" s="24"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="C23" s="14">
         <v>9653</v>
       </c>
-      <c r="D23" s="17">
+      <c r="D23" s="14">
         <v>28231</v>
       </c>
-      <c r="E23" s="2"/>
-      <c r="F23" s="22"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="C24" s="17">
+      <c r="E23" s="23"/>
+      <c r="F23" s="24"/>
+      <c r="H23" s="14">
+        <v>12876</v>
+      </c>
+      <c r="I23" s="14">
+        <v>251481</v>
+      </c>
+      <c r="J23" s="23"/>
+      <c r="K23" s="24"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="C24" s="14">
         <v>9347</v>
       </c>
-      <c r="D24" s="17">
+      <c r="D24" s="14">
         <v>47049</v>
       </c>
-      <c r="E24" s="2"/>
-      <c r="F24" s="22"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="C25" s="17">
+      <c r="E24" s="23"/>
+      <c r="F24" s="24"/>
+      <c r="H24" s="14">
+        <v>14319</v>
+      </c>
+      <c r="I24" s="14">
+        <v>170166</v>
+      </c>
+      <c r="J24" s="23"/>
+      <c r="K24" s="24"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="C25" s="14">
         <v>10066</v>
       </c>
-      <c r="D25" s="17">
+      <c r="D25" s="14">
         <v>31901</v>
       </c>
-      <c r="E25" s="2"/>
-      <c r="F25" s="22"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="23"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A27" s="7"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="24"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A28" s="7"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="24"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A29" s="7"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="24"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A30" s="7"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="24"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A31" s="9"/>
-      <c r="B31" s="9"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="10"/>
+      <c r="E25" s="23"/>
+      <c r="F25" s="24"/>
+      <c r="H25" s="14">
+        <v>13176</v>
+      </c>
+      <c r="I25" s="14">
+        <v>189461</v>
+      </c>
+      <c r="J25" s="23"/>
+      <c r="K25" s="24"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="21"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="22"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="22"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="22"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="22"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A31" s="6"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
+    <mergeCell ref="K20:K25"/>
     <mergeCell ref="E26:E30"/>
     <mergeCell ref="F26:F30"/>
     <mergeCell ref="E20:E25"/>
     <mergeCell ref="F20:F25"/>
+    <mergeCell ref="J20:J25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
results of ex2 30 tasks
</commit_message>
<xml_diff>
--- a/lab4/results.xlsx
+++ b/lab4/results.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7178"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7178" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="experiment1" sheetId="1" r:id="rId1"/>
+    <sheet name="experiment2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="5">
   <si>
     <t>pmin</t>
   </si>
@@ -36,9 +37,6 @@
   </si>
   <si>
     <t>moyenne</t>
-  </si>
-  <si>
-    <t>var</t>
   </si>
   <si>
     <t>pold</t>
@@ -471,8 +469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -486,7 +484,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -498,7 +496,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G1">
         <v>30</v>
@@ -513,7 +511,7 @@
         <v>3</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.45">
@@ -1085,4 +1083,527 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="6" max="6" width="10.6640625" style="3"/>
+    <col min="7" max="7" width="4" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1">
+        <v>30</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A2" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4" t="e">
+        <f>AVERAGE(C2:C7)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F2" s="17" t="e">
+        <f>AVERAGE(D2:D7)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H2" s="4">
+        <v>18036</v>
+      </c>
+      <c r="I2" s="4">
+        <v>70139</v>
+      </c>
+      <c r="J2" s="4">
+        <f>AVERAGE(H2:H7)</f>
+        <v>19897.333333333332</v>
+      </c>
+      <c r="K2" s="17">
+        <f>AVERAGE(I2:I7)</f>
+        <v>62573.666666666664</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="13"/>
+      <c r="H3" s="5">
+        <v>23408</v>
+      </c>
+      <c r="I3" s="5">
+        <v>33315</v>
+      </c>
+      <c r="J3" s="5"/>
+      <c r="K3" s="13"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="13"/>
+      <c r="H4" s="5">
+        <v>21877</v>
+      </c>
+      <c r="I4" s="5">
+        <v>22549</v>
+      </c>
+      <c r="J4" s="5"/>
+      <c r="K4" s="13"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="13"/>
+      <c r="H5" s="14">
+        <v>18718</v>
+      </c>
+      <c r="I5" s="14">
+        <v>99876</v>
+      </c>
+      <c r="J5" s="5"/>
+      <c r="K5" s="13"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="13"/>
+      <c r="H6" s="14">
+        <v>18543</v>
+      </c>
+      <c r="I6" s="14">
+        <v>95819</v>
+      </c>
+      <c r="J6" s="5"/>
+      <c r="K6" s="13"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="7"/>
+      <c r="H7" s="6">
+        <v>18802</v>
+      </c>
+      <c r="I7" s="6">
+        <v>53744</v>
+      </c>
+      <c r="J7" s="6"/>
+      <c r="K7" s="7"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>0.5</v>
+      </c>
+      <c r="B8">
+        <v>0.3</v>
+      </c>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" t="e">
+        <f>AVERAGE(C8:C13)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F8" s="17" t="e">
+        <f>AVERAGE(D8:D13)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H8" s="14">
+        <v>13486</v>
+      </c>
+      <c r="I8" s="14">
+        <v>159510</v>
+      </c>
+      <c r="J8">
+        <f>AVERAGE(H8:H13)</f>
+        <v>17403.666666666668</v>
+      </c>
+      <c r="K8" s="17">
+        <f>AVERAGE(I8:I13)</f>
+        <v>87360.333333333328</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="H9" s="14">
+        <v>18314</v>
+      </c>
+      <c r="I9" s="14">
+        <v>66751</v>
+      </c>
+      <c r="K9" s="3"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="H10" s="14">
+        <v>17820</v>
+      </c>
+      <c r="I10" s="14">
+        <v>65164</v>
+      </c>
+      <c r="K10" s="3"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="H11" s="14">
+        <v>16835</v>
+      </c>
+      <c r="I11" s="14">
+        <v>78205</v>
+      </c>
+      <c r="K11" s="3"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="H12" s="14">
+        <v>19209</v>
+      </c>
+      <c r="I12" s="14">
+        <v>85517</v>
+      </c>
+      <c r="K12" s="3"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="H13" s="14">
+        <v>18758</v>
+      </c>
+      <c r="I13" s="14">
+        <v>69015</v>
+      </c>
+      <c r="K13" s="3"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A14" s="8">
+        <v>0.3</v>
+      </c>
+      <c r="B14" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="15" t="e">
+        <f>AVERAGE(C14:C19)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F14" s="17" t="e">
+        <f>AVERAGE(D14:D19)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H14" s="4">
+        <v>18257</v>
+      </c>
+      <c r="I14" s="4">
+        <v>61657</v>
+      </c>
+      <c r="J14" s="15">
+        <f>AVERAGE(H14:H19)</f>
+        <v>16405.166666666668</v>
+      </c>
+      <c r="K14" s="17">
+        <f>AVERAGE(I14:I19)</f>
+        <v>182547.83333333334</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="18"/>
+      <c r="H15" s="14">
+        <v>16379</v>
+      </c>
+      <c r="I15" s="14">
+        <v>110294</v>
+      </c>
+      <c r="J15" s="16"/>
+      <c r="K15" s="18"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="18"/>
+      <c r="H16" s="14">
+        <v>14885</v>
+      </c>
+      <c r="I16" s="14">
+        <v>302021</v>
+      </c>
+      <c r="J16" s="16"/>
+      <c r="K16" s="18"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="10"/>
+      <c r="H17" s="14">
+        <v>12543</v>
+      </c>
+      <c r="I17" s="14">
+        <v>302020</v>
+      </c>
+      <c r="J17" s="9"/>
+      <c r="K17" s="10"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="10"/>
+      <c r="H18" s="14">
+        <v>16485</v>
+      </c>
+      <c r="I18" s="14">
+        <v>131320</v>
+      </c>
+      <c r="J18" s="9"/>
+      <c r="K18" s="10"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="12"/>
+      <c r="H19" s="6">
+        <v>19882</v>
+      </c>
+      <c r="I19" s="6">
+        <v>187975</v>
+      </c>
+      <c r="J19" s="11"/>
+      <c r="K19" s="12"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A20">
+        <v>0.4</v>
+      </c>
+      <c r="B20">
+        <v>0.4</v>
+      </c>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="23" t="e">
+        <f>AVERAGE(C20:C25)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F20" s="24" t="e">
+        <f>AVERAGE(D20:D25)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H20" s="14">
+        <v>20159</v>
+      </c>
+      <c r="I20" s="14">
+        <v>54902</v>
+      </c>
+      <c r="J20" s="23">
+        <f>AVERAGE(H20:H25)</f>
+        <v>18202.5</v>
+      </c>
+      <c r="K20" s="24">
+        <f>AVERAGE(I20:I25)</f>
+        <v>88736.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="24"/>
+      <c r="H21" s="14">
+        <v>19929</v>
+      </c>
+      <c r="I21" s="14">
+        <v>62572</v>
+      </c>
+      <c r="J21" s="23"/>
+      <c r="K21" s="24"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="24"/>
+      <c r="H22" s="14">
+        <v>21930</v>
+      </c>
+      <c r="I22" s="14">
+        <v>16379</v>
+      </c>
+      <c r="J22" s="23"/>
+      <c r="K22" s="24"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="24"/>
+      <c r="H23" s="14">
+        <v>15286</v>
+      </c>
+      <c r="I23" s="14">
+        <v>167206</v>
+      </c>
+      <c r="J23" s="23"/>
+      <c r="K23" s="24"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="24"/>
+      <c r="H24" s="14">
+        <v>18907</v>
+      </c>
+      <c r="I24" s="14">
+        <v>81267</v>
+      </c>
+      <c r="J24" s="23"/>
+      <c r="K24" s="24"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="23"/>
+      <c r="F25" s="24"/>
+      <c r="H25" s="14">
+        <v>13004</v>
+      </c>
+      <c r="I25" s="14">
+        <v>150093</v>
+      </c>
+      <c r="J25" s="23"/>
+      <c r="K25" s="24"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="21"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="22"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="22"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="22"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="22"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A31" s="6"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="E20:E25"/>
+    <mergeCell ref="F20:F25"/>
+    <mergeCell ref="J20:J25"/>
+    <mergeCell ref="K20:K25"/>
+    <mergeCell ref="E26:E30"/>
+    <mergeCell ref="F26:F30"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>